<commit_message>
2 Months Worth of Changes
Added Clean Version of Code and Graphics generation
</commit_message>
<xml_diff>
--- a/StackedGraphBestNew.xlsx
+++ b/StackedGraphBestNew.xlsx
@@ -427,28 +427,28 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>131</v>
+        <v>559</v>
       </c>
       <c r="C2">
-        <v>223</v>
+        <v>511</v>
       </c>
       <c r="D2">
-        <v>291</v>
+        <v>424</v>
       </c>
       <c r="E2">
-        <v>337</v>
+        <v>391</v>
       </c>
       <c r="F2">
-        <v>361</v>
+        <v>327</v>
       </c>
       <c r="G2">
-        <v>351</v>
+        <v>280</v>
       </c>
       <c r="H2">
-        <v>317</v>
+        <v>206</v>
       </c>
       <c r="I2">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -459,28 +459,28 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C3">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E3">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I3">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -491,28 +491,28 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="C4">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="D4">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="E4">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F4">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G4">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="H4">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="I4">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -523,28 +523,28 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <v>74</v>
+      </c>
+      <c r="C5">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>29</v>
+      </c>
+      <c r="G5">
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <v>17</v>
+      </c>
+      <c r="I5">
         <v>11</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <v>23</v>
-      </c>
-      <c r="F5">
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <v>24</v>
-      </c>
-      <c r="H5">
-        <v>25</v>
-      </c>
-      <c r="I5">
-        <v>18</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -555,28 +555,28 @@
         <v>5</v>
       </c>
       <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="I6">
         <v>3</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -587,11 +587,11 @@
         <v>6</v>
       </c>
       <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
       <c r="D7">
         <v>1</v>
       </c>
@@ -599,13 +599,13 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -619,16 +619,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -651,31 +651,31 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C9">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D9">
-        <v>143</v>
+        <v>232</v>
       </c>
       <c r="E9">
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="F9">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="G9">
-        <v>529</v>
+        <v>409</v>
       </c>
       <c r="H9">
-        <v>709</v>
+        <v>468</v>
       </c>
       <c r="I9">
-        <v>1010</v>
+        <v>578</v>
       </c>
       <c r="J9">
-        <v>1354</v>
+        <v>682</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -683,31 +683,31 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D10">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E10">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F10">
+        <v>59</v>
+      </c>
+      <c r="G10">
         <v>67</v>
       </c>
-      <c r="G10">
-        <v>90</v>
-      </c>
       <c r="H10">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="I10">
-        <v>136</v>
+        <v>77</v>
       </c>
       <c r="J10">
-        <v>181</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -715,31 +715,31 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H11">
         <v>15</v>
       </c>
       <c r="I11">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -747,31 +747,31 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E12">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F12">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G12">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="H12">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="I12">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="J12">
-        <v>301</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -779,31 +779,31 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E13">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I13">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J13">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>